<commit_message>
Added special abilities which can change attributes such as speed and initiative bonuses. Monks were also added to the list of classes along with two archetypes.
</commit_message>
<xml_diff>
--- a/lib/classes/ChoiceFeatures.xlsx
+++ b/lib/classes/ChoiceFeatures.xlsx
@@ -11,39 +11,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Cleric</t>
   </si>
   <si>
+    <t>Monk</t>
+  </si>
+  <si>
     <t>Rogue</t>
   </si>
   <si>
     <t>2=History/Insight/Medicine/Persuasion/Religion</t>
   </si>
   <si>
+    <t>2=Acrobatics/Athletics/History/Insight/Religion/Stealth</t>
+  </si>
+  <si>
     <t>4=Acrobatics/Athletics/Deception/Insight/Intimidation/Investigation/Perception/Performance/Persuasion/Sleight of Hand/Stealth</t>
   </si>
   <si>
     <t>Mace/*War-hammer=Crossbow, Light/?Simple Weapons</t>
   </si>
   <si>
+    <t>Short-sword/?Simple Weapons</t>
+  </si>
+  <si>
     <t>Rapier/Short-sword=Shortbow/Short-sword=2@Dagger</t>
   </si>
   <si>
     <t>Scale Mail/Leather/*Chain Mail=Shield</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>Leather</t>
   </si>
   <si>
     <t>Priest's Pack/Explorer's Pack=Holy Symbol</t>
   </si>
   <si>
+    <t>Dungeoneer's Pack/Explorer's Pack</t>
+  </si>
+  <si>
     <t>Burglar Pack/Dungeoneer's Pack=Explorer's Pack</t>
   </si>
   <si>
     <t>1=Divine Domain:=classes/cleric/DivineDomains.xlsx</t>
+  </si>
+  <si>
+    <t>3=Monastic Tradition:=classes/monk/Monastic Traditions.xlsx</t>
   </si>
   <si>
     <t>3=Roguish Archetype:=classes/rogue/RoguishArchetypes.xlsx</t>
@@ -310,45 +328,63 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>